<commit_message>
feat: Add 2018 data to spreadsheet for reference, continue analysis
</commit_message>
<xml_diff>
--- a/ResidentVNonResident/Data/NatlHuntingLicenseReportFY2019.xlsx
+++ b/ResidentVNonResident/Data/NatlHuntingLicenseReportFY2019.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/GitHub/DataScienceforConservation/ResidentVNonResident/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB6E9D9-7DE5-0D4B-9EB8-5E115E64A0A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBA4350-EA71-254A-9287-E7E93833E825}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{47E855AF-8B85-5B48-A9FD-AAB15C931498}"/>
+    <workbookView xWindow="6840" yWindow="780" windowWidth="27640" windowHeight="16940" xr2:uid="{47E855AF-8B85-5B48-A9FD-AAB15C931498}"/>
   </bookViews>
   <sheets>
     <sheet name="2019-Full" sheetId="1" r:id="rId1"/>
+    <sheet name="2018-Full" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="70">
   <si>
     <t>State</t>
   </si>
@@ -562,15 +563,78 @@
   <si>
     <t>Percent Non-Resident Cost</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>State</t>
+    </r>
+  </si>
+  <si>
+    <t>2018 Paid Hunting License Holders</t>
+  </si>
+  <si>
+    <t>2018 Resident Hunting Licenses, Tags, Permits, and Stamps</t>
+  </si>
+  <si>
+    <t>2018 Non-Resident Hunting Licenses, Tags, Permits, and Stamps</t>
+  </si>
+  <si>
+    <t>2018 Total Hunting Licenses, Tags, Permits, and Stamps</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2018 Cost - Resident Hunting Licenses,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Tags, Permits, and Stamps</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2018 Cost - Non-Resident Hunting Licenses,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Tags, Permits, and Stamps</t>
+    </r>
+  </si>
+  <si>
+    <t>2018 Gross Cost - Hunting Licenses</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -586,6 +650,15 @@
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -621,11 +694,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -644,10 +718,25 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3122873C-BF8A-F04A-9228-78B151C1D644}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{DA274613-8A7D-4F44-90B3-8B9BD7B7AA5C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -961,7 +1050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6256F17E-2D17-7743-BFDF-805E13624CDA}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3169,4 +3260,2165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E10AB5-AC63-7644-9019-EFB0CC56E617}">
+  <dimension ref="A1:M51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="12" width="13.83203125" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>108921</v>
+      </c>
+      <c r="C2" s="11">
+        <v>278248</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2/G2</f>
+        <v>0.78872951981404837</v>
+      </c>
+      <c r="E2" s="11">
+        <v>74532</v>
+      </c>
+      <c r="F2" s="7">
+        <f>E2/G2</f>
+        <v>0.2112704801859516</v>
+      </c>
+      <c r="G2" s="11">
+        <v>352780</v>
+      </c>
+      <c r="H2" s="11">
+        <v>2922692</v>
+      </c>
+      <c r="I2" s="7">
+        <f>H2/L2</f>
+        <v>0.34418653837978341</v>
+      </c>
+      <c r="J2" s="11">
+        <v>5568901</v>
+      </c>
+      <c r="K2" s="7">
+        <f>J2/L2</f>
+        <v>0.65581346162021659</v>
+      </c>
+      <c r="L2" s="12">
+        <v>8491593</v>
+      </c>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>547905</v>
+      </c>
+      <c r="C3" s="11">
+        <v>542838</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D51" si="0">C3/G3</f>
+        <v>0.9360179603547929</v>
+      </c>
+      <c r="E3" s="11">
+        <v>37106</v>
+      </c>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F51" si="1">E3/G3</f>
+        <v>6.3982039645207128E-2</v>
+      </c>
+      <c r="G3" s="11">
+        <v>579944</v>
+      </c>
+      <c r="H3" s="11">
+        <v>5693734</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I51" si="2">H3/L3</f>
+        <v>0.48246050422104875</v>
+      </c>
+      <c r="J3" s="11">
+        <v>6107717</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" ref="K3:K51" si="3">J3/L3</f>
+        <v>0.5175394957789512</v>
+      </c>
+      <c r="L3" s="12">
+        <v>11801451</v>
+      </c>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>326559</v>
+      </c>
+      <c r="C4" s="11">
+        <v>380102</v>
+      </c>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.73514155413638249</v>
+      </c>
+      <c r="E4" s="11">
+        <v>136944</v>
+      </c>
+      <c r="F4" s="7">
+        <f t="shared" si="1"/>
+        <v>0.26485844586361756</v>
+      </c>
+      <c r="G4" s="11">
+        <v>517046</v>
+      </c>
+      <c r="H4" s="11">
+        <v>8186097</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="2"/>
+        <v>0.4362308270003965</v>
+      </c>
+      <c r="J4" s="11">
+        <v>10579420</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="3"/>
+        <v>0.5637691729996035</v>
+      </c>
+      <c r="L4" s="12">
+        <v>18765517</v>
+      </c>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>305214</v>
+      </c>
+      <c r="C5" s="11">
+        <v>456140</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.88100945056176083</v>
+      </c>
+      <c r="E5" s="11">
+        <v>61607</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11899054943823914</v>
+      </c>
+      <c r="G5" s="11">
+        <v>517747</v>
+      </c>
+      <c r="H5" s="11">
+        <v>13358303</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="2"/>
+        <v>0.747355990234576</v>
+      </c>
+      <c r="J5" s="11">
+        <v>4515780</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="3"/>
+        <v>0.25264400976542406</v>
+      </c>
+      <c r="L5" s="12">
+        <v>17874083</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>280967</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1007422</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.97792770055137068</v>
+      </c>
+      <c r="E6" s="11">
+        <v>22738</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="1"/>
+        <v>2.2072299448629339E-2</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1030160</v>
+      </c>
+      <c r="H6" s="11">
+        <v>20609712</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="2"/>
+        <v>0.95344734089026861</v>
+      </c>
+      <c r="J6" s="11">
+        <v>1006282</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="3"/>
+        <v>4.6552659109731435E-2</v>
+      </c>
+      <c r="L6" s="12">
+        <v>21615994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>294319</v>
+      </c>
+      <c r="C7" s="11">
+        <v>459518</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8079238489074555</v>
+      </c>
+      <c r="E7" s="11">
+        <v>109246</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.19207615109254453</v>
+      </c>
+      <c r="G7" s="11">
+        <v>568764</v>
+      </c>
+      <c r="H7" s="11">
+        <v>12751122</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="2"/>
+        <v>0.22348200063463303</v>
+      </c>
+      <c r="J7" s="11">
+        <v>44305473</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="3"/>
+        <v>0.77651799936536692</v>
+      </c>
+      <c r="L7" s="12">
+        <v>57056595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>37489</v>
+      </c>
+      <c r="C8" s="11">
+        <v>124169</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.96831524112546008</v>
+      </c>
+      <c r="E8" s="11">
+        <v>4063</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>3.1684758874539899E-2</v>
+      </c>
+      <c r="G8" s="11">
+        <v>128232</v>
+      </c>
+      <c r="H8" s="11">
+        <v>2085367</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="2"/>
+        <v>0.84076632140165952</v>
+      </c>
+      <c r="J8" s="11">
+        <v>394950</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="3"/>
+        <v>0.15923367859834045</v>
+      </c>
+      <c r="L8" s="12">
+        <v>2480317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>17847</v>
+      </c>
+      <c r="C9" s="11">
+        <v>52315</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.88013122476446837</v>
+      </c>
+      <c r="E9" s="11">
+        <v>7125</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11986877523553163</v>
+      </c>
+      <c r="G9" s="11">
+        <v>59440</v>
+      </c>
+      <c r="H9" s="11">
+        <v>632742</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="2"/>
+        <v>0.62946625759547314</v>
+      </c>
+      <c r="J9" s="11">
+        <v>372462</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="3"/>
+        <v>0.37053374240452686</v>
+      </c>
+      <c r="L9" s="12">
+        <v>1005204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>190232</v>
+      </c>
+      <c r="C10" s="11">
+        <v>313554</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94526829238881072</v>
+      </c>
+      <c r="E10" s="11">
+        <v>18155</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="1"/>
+        <v>5.4731707611189326E-2</v>
+      </c>
+      <c r="G10" s="11">
+        <v>331709</v>
+      </c>
+      <c r="H10" s="11">
+        <v>7890888</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="2"/>
+        <v>0.88912225565100933</v>
+      </c>
+      <c r="J10" s="11">
+        <v>984031</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="3"/>
+        <v>0.11087774434899068</v>
+      </c>
+      <c r="L10" s="12">
+        <v>8874919</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>651910</v>
+      </c>
+      <c r="C11" s="11">
+        <v>1297350</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.88650652810738528</v>
+      </c>
+      <c r="E11" s="11">
+        <v>166091</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11349347189261473</v>
+      </c>
+      <c r="G11" s="11">
+        <v>1463441</v>
+      </c>
+      <c r="H11" s="11">
+        <v>6627327</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="2"/>
+        <v>0.48164536240262823</v>
+      </c>
+      <c r="J11" s="11">
+        <v>7132438</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="3"/>
+        <v>0.51835463759737177</v>
+      </c>
+      <c r="L11" s="12">
+        <v>13759765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11">
+        <v>10617</v>
+      </c>
+      <c r="C12" s="11">
+        <v>11068</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.93780715133028303</v>
+      </c>
+      <c r="E12" s="8">
+        <v>734</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="1"/>
+        <v>6.2192848669716999E-2</v>
+      </c>
+      <c r="G12" s="11">
+        <v>11802</v>
+      </c>
+      <c r="H12" s="11">
+        <v>501285</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="2"/>
+        <v>0.86674274450813082</v>
+      </c>
+      <c r="J12" s="11">
+        <v>77070</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="3"/>
+        <v>0.13325725549186918</v>
+      </c>
+      <c r="L12" s="12">
+        <v>578355</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11">
+        <v>223232</v>
+      </c>
+      <c r="C13" s="11">
+        <v>516446</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.88450103102671074</v>
+      </c>
+      <c r="E13" s="11">
+        <v>67438</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11549896897328922</v>
+      </c>
+      <c r="G13" s="11">
+        <v>583884</v>
+      </c>
+      <c r="H13" s="11">
+        <v>10772431</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="2"/>
+        <v>0.60815645638498084</v>
+      </c>
+      <c r="J13" s="11">
+        <v>6940825</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="3"/>
+        <v>0.39184354361501916</v>
+      </c>
+      <c r="L13" s="12">
+        <v>17713256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11">
+        <v>286947</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1047773</v>
+      </c>
+      <c r="D14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.86808252216036996</v>
+      </c>
+      <c r="E14" s="11">
+        <v>159224</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.13191747783963009</v>
+      </c>
+      <c r="G14" s="11">
+        <v>1206997</v>
+      </c>
+      <c r="H14" s="11">
+        <v>10454861</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="2"/>
+        <v>0.40750571187945811</v>
+      </c>
+      <c r="J14" s="11">
+        <v>15200880</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="3"/>
+        <v>0.59249428812054195</v>
+      </c>
+      <c r="L14" s="12">
+        <v>25655741</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11">
+        <v>306024</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1203507</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.93546604359627272</v>
+      </c>
+      <c r="E15" s="11">
+        <v>83025</v>
+      </c>
+      <c r="F15" s="7">
+        <f t="shared" si="1"/>
+        <v>6.4533956403727236E-2</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1286532</v>
+      </c>
+      <c r="H15" s="11">
+        <v>16424426</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="2"/>
+        <v>0.5141435423114229</v>
+      </c>
+      <c r="J15" s="11">
+        <v>15520789</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="3"/>
+        <v>0.48585645768857716</v>
+      </c>
+      <c r="L15" s="12">
+        <v>31945215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11">
+        <v>267447</v>
+      </c>
+      <c r="C16" s="11">
+        <v>383958</v>
+      </c>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94865580040470521</v>
+      </c>
+      <c r="E16" s="11">
+        <v>20781</v>
+      </c>
+      <c r="F16" s="7">
+        <f t="shared" si="1"/>
+        <v>5.1344199595294744E-2</v>
+      </c>
+      <c r="G16" s="11">
+        <v>404739</v>
+      </c>
+      <c r="H16" s="11">
+        <v>9358292</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.80264991429547972</v>
+      </c>
+      <c r="J16" s="11">
+        <v>2300953</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="3"/>
+        <v>0.19735008570452031</v>
+      </c>
+      <c r="L16" s="12">
+        <v>11659245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11">
+        <v>251390</v>
+      </c>
+      <c r="C17" s="11">
+        <v>349199</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.67169800432796345</v>
+      </c>
+      <c r="E17" s="11">
+        <v>170676</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32830199567203655</v>
+      </c>
+      <c r="G17" s="11">
+        <v>519875</v>
+      </c>
+      <c r="H17" s="11">
+        <v>6732462</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="2"/>
+        <v>0.34638042885251813</v>
+      </c>
+      <c r="J17" s="11">
+        <v>12704150</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="3"/>
+        <v>0.65361957114748193</v>
+      </c>
+      <c r="L17" s="12">
+        <v>19436612</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11">
+        <v>352408</v>
+      </c>
+      <c r="C18" s="11">
+        <v>512113</v>
+      </c>
+      <c r="D18" s="7">
+        <f t="shared" si="0"/>
+        <v>0.83305354116035668</v>
+      </c>
+      <c r="E18" s="11">
+        <v>102629</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" si="1"/>
+        <v>0.16694645883964329</v>
+      </c>
+      <c r="G18" s="11">
+        <v>614742</v>
+      </c>
+      <c r="H18" s="11">
+        <v>12059992</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="2"/>
+        <v>0.60947308792979193</v>
+      </c>
+      <c r="J18" s="11">
+        <v>7727579</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="3"/>
+        <v>0.39052691207020812</v>
+      </c>
+      <c r="L18" s="12">
+        <v>19787571</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11">
+        <v>398808</v>
+      </c>
+      <c r="C19" s="11">
+        <v>605336</v>
+      </c>
+      <c r="D19" s="7">
+        <f t="shared" si="0"/>
+        <v>0.91904308602782325</v>
+      </c>
+      <c r="E19" s="11">
+        <v>53323</v>
+      </c>
+      <c r="F19" s="7">
+        <f t="shared" si="1"/>
+        <v>8.0956913972176803E-2</v>
+      </c>
+      <c r="G19" s="11">
+        <v>658659</v>
+      </c>
+      <c r="H19" s="11">
+        <v>7954155</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="2"/>
+        <v>0.79557509236352808</v>
+      </c>
+      <c r="J19" s="11">
+        <v>2043839</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="3"/>
+        <v>0.20442490763647186</v>
+      </c>
+      <c r="L19" s="12">
+        <v>9997994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11">
+        <v>57921</v>
+      </c>
+      <c r="C20" s="11">
+        <v>246052</v>
+      </c>
+      <c r="D20" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94072397498050131</v>
+      </c>
+      <c r="E20" s="11">
+        <v>15504</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="1"/>
+        <v>5.927602501949869E-2</v>
+      </c>
+      <c r="G20" s="11">
+        <v>261556</v>
+      </c>
+      <c r="H20" s="11">
+        <v>2009739</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="2"/>
+        <v>0.83526966505077105</v>
+      </c>
+      <c r="J20" s="11">
+        <v>396357</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="3"/>
+        <v>0.16473033494922895</v>
+      </c>
+      <c r="L20" s="12">
+        <v>2406096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11">
+        <v>120334</v>
+      </c>
+      <c r="C21" s="11">
+        <v>284941</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8254111253697014</v>
+      </c>
+      <c r="E21" s="11">
+        <v>60270</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.17458887463029857</v>
+      </c>
+      <c r="G21" s="11">
+        <v>345211</v>
+      </c>
+      <c r="H21" s="11">
+        <v>3394548</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="2"/>
+        <v>0.53297547782236321</v>
+      </c>
+      <c r="J21" s="11">
+        <v>2974503</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="3"/>
+        <v>0.46702452217763685</v>
+      </c>
+      <c r="L21" s="12">
+        <v>6369051</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11">
+        <v>163191</v>
+      </c>
+      <c r="C22" s="11">
+        <v>214767</v>
+      </c>
+      <c r="D22" s="7">
+        <f t="shared" si="0"/>
+        <v>0.8622064314103336</v>
+      </c>
+      <c r="E22" s="11">
+        <v>34323</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="1"/>
+        <v>0.13779356858966638</v>
+      </c>
+      <c r="G22" s="11">
+        <v>249090</v>
+      </c>
+      <c r="H22" s="11">
+        <v>4635181</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="2"/>
+        <v>0.58883525566457084</v>
+      </c>
+      <c r="J22" s="11">
+        <v>3236598</v>
+      </c>
+      <c r="K22" s="7">
+        <f t="shared" si="3"/>
+        <v>0.41116474433542916</v>
+      </c>
+      <c r="L22" s="12">
+        <v>7871779</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11">
+        <v>706101</v>
+      </c>
+      <c r="C23" s="11">
+        <v>2171384</v>
+      </c>
+      <c r="D23" s="7">
+        <f t="shared" si="0"/>
+        <v>0.97626710188519761</v>
+      </c>
+      <c r="E23" s="11">
+        <v>52786</v>
+      </c>
+      <c r="F23" s="7">
+        <f t="shared" si="1"/>
+        <v>2.3732898114802375E-2</v>
+      </c>
+      <c r="G23" s="11">
+        <v>2224170</v>
+      </c>
+      <c r="H23" s="11">
+        <v>33009073</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="2"/>
+        <v>0.89081816754447507</v>
+      </c>
+      <c r="J23" s="11">
+        <v>4045709</v>
+      </c>
+      <c r="K23" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1091818324555249</v>
+      </c>
+      <c r="L23" s="12">
+        <v>37054782</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11">
+        <v>568057</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1376759</v>
+      </c>
+      <c r="D24" s="7">
+        <f t="shared" si="0"/>
+        <v>0.96886356407160013</v>
+      </c>
+      <c r="E24" s="11">
+        <v>44245</v>
+      </c>
+      <c r="F24" s="7">
+        <f t="shared" si="1"/>
+        <v>3.113643592839992E-2</v>
+      </c>
+      <c r="G24" s="11">
+        <v>1421004</v>
+      </c>
+      <c r="H24" s="11">
+        <v>27229500</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="2"/>
+        <v>0.88622769068777285</v>
+      </c>
+      <c r="J24" s="11">
+        <v>3495674</v>
+      </c>
+      <c r="K24" s="7">
+        <f t="shared" si="3"/>
+        <v>0.11377230931222716</v>
+      </c>
+      <c r="L24" s="12">
+        <v>30725174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11">
+        <v>498319</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1702400</v>
+      </c>
+      <c r="D25" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9551601032138467</v>
+      </c>
+      <c r="E25" s="11">
+        <v>79919</v>
+      </c>
+      <c r="F25" s="7">
+        <f t="shared" si="1"/>
+        <v>4.483989678615332E-2</v>
+      </c>
+      <c r="G25" s="11">
+        <v>1782319</v>
+      </c>
+      <c r="H25" s="11">
+        <v>12585185</v>
+      </c>
+      <c r="I25" s="7">
+        <f t="shared" si="2"/>
+        <v>0.59102468131628683</v>
+      </c>
+      <c r="J25" s="11">
+        <v>8708655</v>
+      </c>
+      <c r="K25" s="7">
+        <f t="shared" si="3"/>
+        <v>0.40897531868371323</v>
+      </c>
+      <c r="L25" s="12">
+        <v>21293840</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11">
+        <v>300146</v>
+      </c>
+      <c r="C26" s="11">
+        <v>335324</v>
+      </c>
+      <c r="D26" s="7">
+        <f t="shared" si="0"/>
+        <v>0.7858063488046193</v>
+      </c>
+      <c r="E26" s="11">
+        <v>91402</v>
+      </c>
+      <c r="F26" s="7">
+        <f t="shared" si="1"/>
+        <v>0.21419365119538064</v>
+      </c>
+      <c r="G26" s="11">
+        <v>426726</v>
+      </c>
+      <c r="H26" s="11">
+        <v>4023594</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="2"/>
+        <v>0.32785017039092013</v>
+      </c>
+      <c r="J26" s="11">
+        <v>8249067</v>
+      </c>
+      <c r="K26" s="7">
+        <f t="shared" si="3"/>
+        <v>0.67214982960907987</v>
+      </c>
+      <c r="L26" s="12">
+        <v>12272661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11">
+        <v>253412</v>
+      </c>
+      <c r="C27" s="11">
+        <v>873323</v>
+      </c>
+      <c r="D27" s="7">
+        <f t="shared" si="0"/>
+        <v>0.84872606977193943</v>
+      </c>
+      <c r="E27" s="11">
+        <v>155658</v>
+      </c>
+      <c r="F27" s="7">
+        <f t="shared" si="1"/>
+        <v>0.15127393022806057</v>
+      </c>
+      <c r="G27" s="11">
+        <v>1028981</v>
+      </c>
+      <c r="H27" s="11">
+        <v>9459094</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="2"/>
+        <v>0.28735578165540016</v>
+      </c>
+      <c r="J27" s="11">
+        <v>23458615</v>
+      </c>
+      <c r="K27" s="7">
+        <f t="shared" si="3"/>
+        <v>0.7126442183445999</v>
+      </c>
+      <c r="L27" s="12">
+        <v>32917709</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11">
+        <v>585766</v>
+      </c>
+      <c r="C28" s="11">
+        <v>319136</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" si="0"/>
+        <v>0.92567046252197172</v>
+      </c>
+      <c r="E28" s="11">
+        <v>25626</v>
+      </c>
+      <c r="F28" s="7">
+        <f t="shared" si="1"/>
+        <v>7.4329537478028326E-2</v>
+      </c>
+      <c r="G28" s="11">
+        <v>344762</v>
+      </c>
+      <c r="H28" s="11">
+        <v>8629779</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="2"/>
+        <v>0.80219449968645751</v>
+      </c>
+      <c r="J28" s="11">
+        <v>2127935</v>
+      </c>
+      <c r="K28" s="7">
+        <f t="shared" si="3"/>
+        <v>0.19780550031354244</v>
+      </c>
+      <c r="L28" s="12">
+        <v>10757714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="11">
+        <v>141553</v>
+      </c>
+      <c r="C29" s="11">
+        <v>362554</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" si="0"/>
+        <v>0.69674356929403969</v>
+      </c>
+      <c r="E29" s="11">
+        <v>157801</v>
+      </c>
+      <c r="F29" s="7">
+        <f t="shared" si="1"/>
+        <v>0.30325643070596037</v>
+      </c>
+      <c r="G29" s="11">
+        <v>520355</v>
+      </c>
+      <c r="H29" s="11">
+        <v>4257890</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="2"/>
+        <v>0.36049459646294696</v>
+      </c>
+      <c r="J29" s="11">
+        <v>7553355</v>
+      </c>
+      <c r="K29" s="7">
+        <f t="shared" si="3"/>
+        <v>0.63950540353705299</v>
+      </c>
+      <c r="L29" s="12">
+        <v>11811245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11">
+        <v>183056</v>
+      </c>
+      <c r="C30" s="11">
+        <v>339053</v>
+      </c>
+      <c r="D30" s="7">
+        <f t="shared" si="0"/>
+        <v>0.78986383385167325</v>
+      </c>
+      <c r="E30" s="11">
+        <v>90202</v>
+      </c>
+      <c r="F30" s="7">
+        <f t="shared" si="1"/>
+        <v>0.21013616614832675</v>
+      </c>
+      <c r="G30" s="11">
+        <v>429255</v>
+      </c>
+      <c r="H30" s="11">
+        <v>7565754</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="2"/>
+        <v>0.56036557821409105</v>
+      </c>
+      <c r="J30" s="11">
+        <v>5935707</v>
+      </c>
+      <c r="K30" s="7">
+        <f t="shared" si="3"/>
+        <v>0.43963442178590895</v>
+      </c>
+      <c r="L30" s="12">
+        <v>13501461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="11">
+        <v>58099</v>
+      </c>
+      <c r="C31" s="11">
+        <v>186931</v>
+      </c>
+      <c r="D31" s="7">
+        <f t="shared" si="0"/>
+        <v>0.85613853495891767</v>
+      </c>
+      <c r="E31" s="11">
+        <v>31411</v>
+      </c>
+      <c r="F31" s="7">
+        <f t="shared" si="1"/>
+        <v>0.14386146504108233</v>
+      </c>
+      <c r="G31" s="11">
+        <v>218342</v>
+      </c>
+      <c r="H31" s="11">
+        <v>2646432</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="2"/>
+        <v>0.65875116090295416</v>
+      </c>
+      <c r="J31" s="11">
+        <v>1370915</v>
+      </c>
+      <c r="K31" s="7">
+        <f t="shared" si="3"/>
+        <v>0.3412488390970459</v>
+      </c>
+      <c r="L31" s="12">
+        <v>4017347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="11">
+        <v>74794</v>
+      </c>
+      <c r="C32" s="11">
+        <v>303795</v>
+      </c>
+      <c r="D32" s="7">
+        <f t="shared" si="0"/>
+        <v>0.71948929155900598</v>
+      </c>
+      <c r="E32" s="11">
+        <v>118442</v>
+      </c>
+      <c r="F32" s="7">
+        <f t="shared" si="1"/>
+        <v>0.28051070844099402</v>
+      </c>
+      <c r="G32" s="11">
+        <v>422237</v>
+      </c>
+      <c r="H32" s="11">
+        <v>6981229</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="2"/>
+        <v>0.85880908578152326</v>
+      </c>
+      <c r="J32" s="11">
+        <v>1147736</v>
+      </c>
+      <c r="K32" s="7">
+        <f t="shared" si="3"/>
+        <v>0.14119091421847677</v>
+      </c>
+      <c r="L32" s="12">
+        <v>8128965</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="11">
+        <v>107331</v>
+      </c>
+      <c r="C33" s="11">
+        <v>329423</v>
+      </c>
+      <c r="D33" s="7">
+        <f t="shared" si="0"/>
+        <v>0.74545944160070243</v>
+      </c>
+      <c r="E33" s="11">
+        <v>112483</v>
+      </c>
+      <c r="F33" s="7">
+        <f t="shared" si="1"/>
+        <v>0.25454055839929757</v>
+      </c>
+      <c r="G33" s="11">
+        <v>441906</v>
+      </c>
+      <c r="H33" s="11">
+        <v>5866269</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="2"/>
+        <v>0.36243637265894507</v>
+      </c>
+      <c r="J33" s="11">
+        <v>10319383</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="3"/>
+        <v>0.63756362734105487</v>
+      </c>
+      <c r="L33" s="12">
+        <v>16185652</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11">
+        <v>68744</v>
+      </c>
+      <c r="C34" s="11">
+        <v>123271</v>
+      </c>
+      <c r="D34" s="7">
+        <f t="shared" si="0"/>
+        <v>0.82119897942189446</v>
+      </c>
+      <c r="E34" s="11">
+        <v>26840</v>
+      </c>
+      <c r="F34" s="7">
+        <f t="shared" si="1"/>
+        <v>0.17880102057810554</v>
+      </c>
+      <c r="G34" s="11">
+        <v>150111</v>
+      </c>
+      <c r="H34" s="11">
+        <v>3920404</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="2"/>
+        <v>0.50583351741023408</v>
+      </c>
+      <c r="J34" s="11">
+        <v>3829980</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="3"/>
+        <v>0.49416648258976587</v>
+      </c>
+      <c r="L34" s="12">
+        <v>7750384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11">
+        <v>579043</v>
+      </c>
+      <c r="C35" s="11">
+        <v>1117576</v>
+      </c>
+      <c r="D35" s="7">
+        <f t="shared" si="0"/>
+        <v>0.95818318530731372</v>
+      </c>
+      <c r="E35" s="11">
+        <v>48773</v>
+      </c>
+      <c r="F35" s="7">
+        <f t="shared" si="1"/>
+        <v>4.1816814692686326E-2</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1166349</v>
+      </c>
+      <c r="H35" s="11">
+        <v>17441081</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="2"/>
+        <v>0.80677408617219415</v>
+      </c>
+      <c r="J35" s="11">
+        <v>4177215</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="3"/>
+        <v>0.19322591382780585</v>
+      </c>
+      <c r="L35" s="12">
+        <v>21618296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="11">
+        <v>390268</v>
+      </c>
+      <c r="C36" s="11">
+        <v>895099</v>
+      </c>
+      <c r="D36" s="7">
+        <f t="shared" si="0"/>
+        <v>0.89944873407800119</v>
+      </c>
+      <c r="E36" s="11">
+        <v>100065</v>
+      </c>
+      <c r="F36" s="7">
+        <f t="shared" si="1"/>
+        <v>0.10055126592199878</v>
+      </c>
+      <c r="G36" s="11">
+        <v>995164</v>
+      </c>
+      <c r="H36" s="11">
+        <v>16259079</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="2"/>
+        <v>0.71822207438790298</v>
+      </c>
+      <c r="J36" s="11">
+        <v>6378876</v>
+      </c>
+      <c r="K36" s="7">
+        <f t="shared" si="3"/>
+        <v>0.28177792561209702</v>
+      </c>
+      <c r="L36" s="12">
+        <v>22637955</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="11">
+        <v>529651</v>
+      </c>
+      <c r="C37" s="11">
+        <v>377498</v>
+      </c>
+      <c r="D37" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94318380563564674</v>
+      </c>
+      <c r="E37" s="11">
+        <v>22740</v>
+      </c>
+      <c r="F37" s="7">
+        <f t="shared" si="1"/>
+        <v>5.6816194364353208E-2</v>
+      </c>
+      <c r="G37" s="11">
+        <v>400238</v>
+      </c>
+      <c r="H37" s="11">
+        <v>5735625</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="2"/>
+        <v>0.59706612752317534</v>
+      </c>
+      <c r="J37" s="11">
+        <v>3870723</v>
+      </c>
+      <c r="K37" s="7">
+        <f t="shared" si="3"/>
+        <v>0.40293387247682472</v>
+      </c>
+      <c r="L37" s="12">
+        <v>9606348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="11">
+        <v>264684</v>
+      </c>
+      <c r="C38" s="11">
+        <v>1173427</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" si="0"/>
+        <v>0.95972502801246451</v>
+      </c>
+      <c r="E38" s="11">
+        <v>49243</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" si="1"/>
+        <v>4.0274971987535477E-2</v>
+      </c>
+      <c r="G38" s="11">
+        <v>1222670</v>
+      </c>
+      <c r="H38" s="11">
+        <v>20982703</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="2"/>
+        <v>0.79481522225841406</v>
+      </c>
+      <c r="J38" s="11">
+        <v>5416770</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="3"/>
+        <v>0.20518477774158597</v>
+      </c>
+      <c r="L38" s="12">
+        <v>26399473</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="11">
+        <v>975650</v>
+      </c>
+      <c r="C39" s="11">
+        <v>2468652</v>
+      </c>
+      <c r="D39" s="7">
+        <f t="shared" si="0"/>
+        <v>0.96059114450588146</v>
+      </c>
+      <c r="E39" s="11">
+        <v>101278</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="1"/>
+        <v>3.9408855494118517E-2</v>
+      </c>
+      <c r="G39" s="11">
+        <v>2569930</v>
+      </c>
+      <c r="H39" s="11">
+        <v>30352406</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="2"/>
+        <v>0.83312909792912881</v>
+      </c>
+      <c r="J39" s="11">
+        <v>6079410</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="3"/>
+        <v>0.16687090207087124</v>
+      </c>
+      <c r="L39" s="12">
+        <v>36431816</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="11">
+        <v>8209</v>
+      </c>
+      <c r="C40" s="11">
+        <v>26515</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" si="0"/>
+        <v>0.85800731320583767</v>
+      </c>
+      <c r="E40" s="11">
+        <v>4388</v>
+      </c>
+      <c r="F40" s="7">
+        <f t="shared" si="1"/>
+        <v>0.14199268679416238</v>
+      </c>
+      <c r="G40" s="11">
+        <v>30903</v>
+      </c>
+      <c r="H40" s="11">
+        <v>362093</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="2"/>
+        <v>0.74878199083494634</v>
+      </c>
+      <c r="J40" s="11">
+        <v>121483</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" si="3"/>
+        <v>0.25121800916505366</v>
+      </c>
+      <c r="L40" s="12">
+        <v>483576</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="11">
+        <v>210369</v>
+      </c>
+      <c r="C41" s="11">
+        <v>722055</v>
+      </c>
+      <c r="D41" s="7">
+        <f t="shared" si="0"/>
+        <v>0.88673498836402487</v>
+      </c>
+      <c r="E41" s="11">
+        <v>92230</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11326501163597512</v>
+      </c>
+      <c r="G41" s="11">
+        <v>814285</v>
+      </c>
+      <c r="H41" s="11">
+        <v>5434146</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="2"/>
+        <v>0.55922282259364153</v>
+      </c>
+      <c r="J41" s="11">
+        <v>4283172</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="3"/>
+        <v>0.44077717740635841</v>
+      </c>
+      <c r="L41" s="12">
+        <v>9717318</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="11">
+        <v>233215</v>
+      </c>
+      <c r="C42" s="11">
+        <v>245474</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="0"/>
+        <v>0.65638971484801167</v>
+      </c>
+      <c r="E42" s="11">
+        <v>128502</v>
+      </c>
+      <c r="F42" s="7">
+        <f t="shared" si="1"/>
+        <v>0.34361028515198838</v>
+      </c>
+      <c r="G42" s="11">
+        <v>373976</v>
+      </c>
+      <c r="H42" s="11">
+        <v>7186745</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="2"/>
+        <v>0.32575634745415805</v>
+      </c>
+      <c r="J42" s="11">
+        <v>14874974</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="3"/>
+        <v>0.67424365254584195</v>
+      </c>
+      <c r="L42" s="12">
+        <v>22061719</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="11">
+        <v>700600</v>
+      </c>
+      <c r="C43" s="11">
+        <v>696906</v>
+      </c>
+      <c r="D43" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94537645844326912</v>
+      </c>
+      <c r="E43" s="11">
+        <v>40267</v>
+      </c>
+      <c r="F43" s="7">
+        <f t="shared" si="1"/>
+        <v>5.4623541556730916E-2</v>
+      </c>
+      <c r="G43" s="11">
+        <v>737173</v>
+      </c>
+      <c r="H43" s="11">
+        <v>17016820</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="2"/>
+        <v>0.82126784304945566</v>
+      </c>
+      <c r="J43" s="11">
+        <v>3703363</v>
+      </c>
+      <c r="K43" s="7">
+        <f t="shared" si="3"/>
+        <v>0.17873215695054431</v>
+      </c>
+      <c r="L43" s="12">
+        <v>20720183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="11">
+        <v>1157779</v>
+      </c>
+      <c r="C44" s="11">
+        <v>1575985</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="0"/>
+        <v>0.95205948253624773</v>
+      </c>
+      <c r="E44" s="11">
+        <v>79358</v>
+      </c>
+      <c r="F44" s="7">
+        <f t="shared" si="1"/>
+        <v>4.7940517463752226E-2</v>
+      </c>
+      <c r="G44" s="11">
+        <v>1655343</v>
+      </c>
+      <c r="H44" s="11">
+        <v>35200343</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="2"/>
+        <v>0.76161935834064487</v>
+      </c>
+      <c r="J44" s="11">
+        <v>11017420</v>
+      </c>
+      <c r="K44" s="7">
+        <f t="shared" si="3"/>
+        <v>0.23838064165935507</v>
+      </c>
+      <c r="L44" s="12">
+        <v>46217763</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="11">
+        <v>236656</v>
+      </c>
+      <c r="C45" s="11">
+        <v>379805</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="0"/>
+        <v>0.90249048928217546</v>
+      </c>
+      <c r="E45" s="11">
+        <v>41036</v>
+      </c>
+      <c r="F45" s="7">
+        <f t="shared" si="1"/>
+        <v>9.7509510717824543E-2</v>
+      </c>
+      <c r="G45" s="11">
+        <v>420841</v>
+      </c>
+      <c r="H45" s="11">
+        <v>11216469</v>
+      </c>
+      <c r="I45" s="7">
+        <f t="shared" si="2"/>
+        <v>0.66915910453837468</v>
+      </c>
+      <c r="J45" s="11">
+        <v>5545567</v>
+      </c>
+      <c r="K45" s="7">
+        <f t="shared" si="3"/>
+        <v>0.33084089546162532</v>
+      </c>
+      <c r="L45" s="12">
+        <v>16762036</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="11">
+        <v>276019</v>
+      </c>
+      <c r="C46" s="11">
+        <v>815464</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94813126762200972</v>
+      </c>
+      <c r="E46" s="11">
+        <v>44611</v>
+      </c>
+      <c r="F46" s="7">
+        <f t="shared" si="1"/>
+        <v>5.1868732377990293E-2</v>
+      </c>
+      <c r="G46" s="11">
+        <v>860075</v>
+      </c>
+      <c r="H46" s="11">
+        <v>17488685</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="2"/>
+        <v>0.82090211487138209</v>
+      </c>
+      <c r="J46" s="11">
+        <v>3815542</v>
+      </c>
+      <c r="K46" s="7">
+        <f t="shared" si="3"/>
+        <v>0.17909788512861791</v>
+      </c>
+      <c r="L46" s="12">
+        <v>21304227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="11">
+        <v>69943</v>
+      </c>
+      <c r="C47" s="11">
+        <v>153476</v>
+      </c>
+      <c r="D47" s="7">
+        <f t="shared" si="0"/>
+        <v>0.90638287820088825</v>
+      </c>
+      <c r="E47" s="11">
+        <v>15852</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="1"/>
+        <v>9.3617121799111788E-2</v>
+      </c>
+      <c r="G47" s="11">
+        <v>169328</v>
+      </c>
+      <c r="H47" s="11">
+        <v>2975620</v>
+      </c>
+      <c r="I47" s="7">
+        <f t="shared" si="2"/>
+        <v>0.75036659433547137</v>
+      </c>
+      <c r="J47" s="11">
+        <v>989935</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="3"/>
+        <v>0.24963340566452868</v>
+      </c>
+      <c r="L47" s="12">
+        <v>3965555</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="11">
+        <v>183063</v>
+      </c>
+      <c r="C48" s="11">
+        <v>681049</v>
+      </c>
+      <c r="D48" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9845561575870424</v>
+      </c>
+      <c r="E48" s="11">
+        <v>10683</v>
+      </c>
+      <c r="F48" s="7">
+        <f t="shared" si="1"/>
+        <v>1.5443842412957619E-2</v>
+      </c>
+      <c r="G48" s="11">
+        <v>691732</v>
+      </c>
+      <c r="H48" s="11">
+        <v>16129772</v>
+      </c>
+      <c r="I48" s="7">
+        <f t="shared" si="2"/>
+        <v>0.93822151519506991</v>
+      </c>
+      <c r="J48" s="11">
+        <v>1062087</v>
+      </c>
+      <c r="K48" s="7">
+        <f t="shared" si="3"/>
+        <v>6.1778484804930055E-2</v>
+      </c>
+      <c r="L48" s="12">
+        <v>17191859</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="11">
+        <v>706400</v>
+      </c>
+      <c r="C49" s="11">
+        <v>2716899</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" si="0"/>
+        <v>0.94874524911337732</v>
+      </c>
+      <c r="E49" s="11">
+        <v>146777</v>
+      </c>
+      <c r="F49" s="7">
+        <f t="shared" si="1"/>
+        <v>5.1254750886622652E-2</v>
+      </c>
+      <c r="G49" s="11">
+        <v>2863676</v>
+      </c>
+      <c r="H49" s="11">
+        <v>33771619</v>
+      </c>
+      <c r="I49" s="7">
+        <f t="shared" si="2"/>
+        <v>0.81610679800563402</v>
+      </c>
+      <c r="J49" s="11">
+        <v>7609753</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" si="3"/>
+        <v>0.18389320199436596</v>
+      </c>
+      <c r="L49" s="12">
+        <v>41381372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="11">
+        <v>217123</v>
+      </c>
+      <c r="C50" s="11">
+        <v>537767</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" si="0"/>
+        <v>0.79350607191866729</v>
+      </c>
+      <c r="E50" s="11">
+        <v>139943</v>
+      </c>
+      <c r="F50" s="7">
+        <f t="shared" si="1"/>
+        <v>0.20649392808133271</v>
+      </c>
+      <c r="G50" s="11">
+        <v>677710</v>
+      </c>
+      <c r="H50" s="11">
+        <v>4354126</v>
+      </c>
+      <c r="I50" s="7">
+        <f t="shared" si="2"/>
+        <v>0.47209944811284954</v>
+      </c>
+      <c r="J50" s="11">
+        <v>4868774</v>
+      </c>
+      <c r="K50" s="7">
+        <f t="shared" si="3"/>
+        <v>0.52790055188715046</v>
+      </c>
+      <c r="L50" s="12">
+        <v>9222900</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="11">
+        <v>130304</v>
+      </c>
+      <c r="C51" s="11">
+        <v>176549</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" si="0"/>
+        <v>0.71213808014069391</v>
+      </c>
+      <c r="E51" s="11">
+        <v>71365</v>
+      </c>
+      <c r="F51" s="7">
+        <f t="shared" si="1"/>
+        <v>0.28786191985930604</v>
+      </c>
+      <c r="G51" s="11">
+        <v>247914</v>
+      </c>
+      <c r="H51" s="11">
+        <v>6484947</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" si="2"/>
+        <v>0.26072264303598297</v>
+      </c>
+      <c r="J51" s="11">
+        <v>18388025</v>
+      </c>
+      <c r="K51" s="7">
+        <f t="shared" si="3"/>
+        <v>0.73927735696401697</v>
+      </c>
+      <c r="L51" s="12">
+        <v>24872972</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: update license data
</commit_message>
<xml_diff>
--- a/ResidentVNonResident/Data/NatlHuntingLicenseReportFY2019.xlsx
+++ b/ResidentVNonResident/Data/NatlHuntingLicenseReportFY2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherkusmierz/GitHub/DataScienceforConservation/ResidentVNonResident/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBA4350-EA71-254A-9287-E7E93833E825}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604F40D0-8897-704D-AD26-7E283D83D27F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6840" yWindow="780" windowWidth="27640" windowHeight="16940" xr2:uid="{47E855AF-8B85-5B48-A9FD-AAB15C931498}"/>
   </bookViews>
@@ -634,7 +634,7 @@
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -661,13 +661,25 @@
       <name val="Verdana"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -699,7 +711,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -732,6 +744,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="7" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="37" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1051,7 +1075,10 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K51"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3128,44 +3155,44 @@
       <c r="M48" s="5"/>
     </row>
     <row r="49" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B49" s="15">
         <v>692209</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="15">
         <v>418349</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="16">
         <f t="shared" si="0"/>
         <v>0.24428339861587009</v>
       </c>
-      <c r="E49" s="4">
+      <c r="E49" s="15">
         <v>1294207</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="17">
         <f t="shared" si="1"/>
         <v>0.75571660138412988</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="15">
         <v>1712556</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="15">
         <v>11266763</v>
       </c>
-      <c r="I49" s="7">
+      <c r="I49" s="16">
         <f t="shared" si="2"/>
         <v>0.29144971201953601</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49" s="15">
         <v>27390894</v>
       </c>
-      <c r="K49" s="7">
+      <c r="K49" s="16">
         <f t="shared" si="3"/>
         <v>0.70855028798046404</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="15">
         <v>38657657</v>
       </c>
       <c r="M49" s="5"/>
@@ -3267,7 +3294,10 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>